<commit_message>
admin panel issue resolved
</commit_message>
<xml_diff>
--- a/public/uploads/dummy.xlsx
+++ b/public/uploads/dummy.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="FoodSales" sheetId="1" r:id="rId4"/>
+    <sheet name="FoodSales" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgqGRyt8hWL7WWj2YG2gExLzhAEpA=="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Invite Code</t>
   </si>
@@ -49,21 +48,82 @@
   </si>
   <si>
     <t>AAA222</t>
+  </si>
+  <si>
+    <t>Church Name</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>sdsds</t>
+  </si>
+  <si>
+    <t>fdsfd</t>
+  </si>
+  <si>
+    <t>dfds</t>
+  </si>
+  <si>
+    <t>ffdsfs</t>
+  </si>
+  <si>
+    <t>hjk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,38 +131,151 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="1">
     <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -300,87 +473,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7d45038a-e85d-4e87-9ca7-53ed7df586a4}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.635" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.0"/>
-    <col customWidth="1" min="2" max="2" width="5.75"/>
-    <col customWidth="1" min="3" max="3" width="7.5"/>
-    <col customWidth="1" min="4" max="4" width="9.75"/>
-    <col customWidth="1" min="5" max="5" width="9.13"/>
-    <col customWidth="1" min="6" max="7" width="7.63"/>
-    <col customWidth="1" min="8" max="8" width="9.75"/>
-    <col customWidth="1" min="9" max="26" width="7.63"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="5.75" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="5" max="5" width="9.125" customWidth="1"/>
+    <col min="6" max="7" width="7.625" customWidth="1"/>
+    <col min="8" max="8" width="9.75" customWidth="1"/>
+    <col min="9" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7"/>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>